<commit_message>
More updates to simple_window_frame - added close_on feautre
</commit_message>
<xml_diff>
--- a/Docs/Form examples.xlsx
+++ b/Docs/Form examples.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Documents\Code\TaskBarApp\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05732D6-1B34-418F-B82D-72FA1C3ED4A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55438AA7-43CA-4DFA-9E77-8947BCA374E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{13726A4F-0F43-429C-850C-1C3F8B016DD4}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{13726A4F-0F43-429C-850C-1C3F8B016DD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Forms screen shots" sheetId="2" r:id="rId1"/>
     <sheet name="Form def" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -744,24 +745,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -771,7 +769,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
@@ -1018,13 +1015,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>116778</xdr:colOff>
+      <xdr:colOff>48742</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>127411</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
-      <xdr:colOff>79796</xdr:colOff>
+      <xdr:colOff>11760</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>187582</xdr:rowOff>
     </xdr:to>
@@ -1049,8 +1046,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17185578" y="508411"/>
-          <a:ext cx="4234028" cy="2710026"/>
+          <a:off x="18050992" y="3311482"/>
+          <a:ext cx="4249268" cy="2727171"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1737,7 +1734,7 @@
   <dimension ref="A3:AP12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="Z15" sqref="Z15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1745,442 +1742,407 @@
     <col min="1" max="1" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:42" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C3" s="21" t="s">
+    <row r="3" spans="1:42" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C3" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="N3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="U3" s="21" t="s">
+      <c r="U3" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="AC3" s="21" t="s">
+      <c r="AC3" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="AK3" s="21" t="s">
+      <c r="AK3" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:42" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+    <row r="4" spans="1:42" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="N4" s="21" t="s">
+      <c r="N4" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="U4" s="21" t="s">
+      <c r="U4" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AC4" s="21" t="s">
+      <c r="AC4" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="AK4" s="21" t="s">
+      <c r="AK4" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:42" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+    <row r="5" spans="1:42" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23" t="s">
+      <c r="B5" s="20"/>
+      <c r="C5" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23" t="s">
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23" t="s">
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="23"/>
-      <c r="U5" s="23" t="s">
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="20"/>
+      <c r="U5" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="V5" s="23"/>
-      <c r="W5" s="23"/>
-      <c r="X5" s="23"/>
-      <c r="Y5" s="23"/>
-      <c r="Z5" s="23"/>
-      <c r="AA5" s="23"/>
-      <c r="AB5" s="23"/>
-      <c r="AC5" s="23" t="s">
+      <c r="V5" s="20"/>
+      <c r="W5" s="20"/>
+      <c r="X5" s="20"/>
+      <c r="Y5" s="20"/>
+      <c r="Z5" s="20"/>
+      <c r="AA5" s="20"/>
+      <c r="AB5" s="20"/>
+      <c r="AC5" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="AD5" s="23"/>
-      <c r="AE5" s="23"/>
-      <c r="AF5" s="23"/>
-      <c r="AG5" s="23"/>
-      <c r="AH5" s="23"/>
-      <c r="AI5" s="23"/>
-      <c r="AJ5" s="23"/>
-      <c r="AK5" s="23" t="s">
+      <c r="AD5" s="20"/>
+      <c r="AE5" s="20"/>
+      <c r="AF5" s="20"/>
+      <c r="AG5" s="20"/>
+      <c r="AH5" s="20"/>
+      <c r="AI5" s="20"/>
+      <c r="AJ5" s="20"/>
+      <c r="AK5" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="AL5" s="23"/>
-      <c r="AM5" s="23"/>
-      <c r="AN5" s="23"/>
-      <c r="AO5" s="23"/>
-      <c r="AP5" s="23"/>
+      <c r="AL5" s="20"/>
+      <c r="AM5" s="20"/>
+      <c r="AN5" s="20"/>
+      <c r="AO5" s="20"/>
+      <c r="AP5" s="20"/>
     </row>
-    <row r="6" spans="1:42" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+    <row r="6" spans="1:42" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="N6" s="21" t="s">
+      <c r="N6" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="U6" s="21" t="s">
+      <c r="U6" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="AC6" s="21" t="s">
+      <c r="AC6" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="AK6" s="21" t="s">
+      <c r="AK6" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:42" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+    <row r="7" spans="1:42" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="24" t="s">
+      <c r="B7" s="20"/>
+      <c r="C7" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="24" t="s">
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="24" t="s">
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="23"/>
-      <c r="U7" s="25" t="s">
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="20"/>
+      <c r="U7" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="V7" s="23"/>
-      <c r="W7" s="23"/>
-      <c r="X7" s="23"/>
-      <c r="Y7" s="23"/>
-      <c r="Z7" s="23"/>
-      <c r="AA7" s="23"/>
-      <c r="AB7" s="23"/>
-      <c r="AC7" s="25" t="s">
+      <c r="V7" s="20"/>
+      <c r="W7" s="20"/>
+      <c r="X7" s="20"/>
+      <c r="Y7" s="20"/>
+      <c r="Z7" s="20"/>
+      <c r="AA7" s="20"/>
+      <c r="AB7" s="20"/>
+      <c r="AC7" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="AD7" s="23"/>
-      <c r="AE7" s="23"/>
-      <c r="AF7" s="23"/>
-      <c r="AG7" s="23"/>
-      <c r="AH7" s="23"/>
-      <c r="AI7" s="23"/>
-      <c r="AJ7" s="23"/>
-      <c r="AK7" s="25" t="s">
+      <c r="AD7" s="20"/>
+      <c r="AE7" s="20"/>
+      <c r="AF7" s="20"/>
+      <c r="AG7" s="20"/>
+      <c r="AH7" s="20"/>
+      <c r="AI7" s="20"/>
+      <c r="AJ7" s="20"/>
+      <c r="AK7" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="AL7" s="23"/>
-      <c r="AM7" s="23"/>
-      <c r="AN7" s="23"/>
-      <c r="AO7" s="23"/>
-      <c r="AP7" s="23"/>
+      <c r="AL7" s="20"/>
+      <c r="AM7" s="20"/>
+      <c r="AN7" s="20"/>
+      <c r="AO7" s="20"/>
+      <c r="AP7" s="20"/>
     </row>
-    <row r="8" spans="1:42" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+    <row r="8" spans="1:42" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="23" t="s">
+      <c r="N8" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="O8" s="26"/>
-      <c r="P8" s="26"/>
-      <c r="Q8" s="26"/>
-      <c r="R8" s="26"/>
-      <c r="S8" s="26"/>
-      <c r="T8" s="26"/>
-      <c r="U8" s="23" t="s">
+      <c r="U8" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="V8" s="26"/>
-      <c r="W8" s="26"/>
-      <c r="X8" s="26"/>
-      <c r="Y8" s="26"/>
-      <c r="Z8" s="26"/>
-      <c r="AA8" s="26"/>
-      <c r="AB8" s="26"/>
-      <c r="AC8" s="26" t="s">
+      <c r="AC8" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="AD8" s="26"/>
-      <c r="AE8" s="26"/>
-      <c r="AF8" s="26"/>
-      <c r="AG8" s="26"/>
-      <c r="AH8" s="26"/>
-      <c r="AI8" s="26"/>
-      <c r="AJ8" s="26"/>
-      <c r="AK8" s="26" t="s">
+      <c r="AK8" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="AL8" s="26"/>
-      <c r="AM8" s="26"/>
-      <c r="AN8" s="26"/>
-      <c r="AO8" s="26"/>
-      <c r="AP8" s="26"/>
     </row>
-    <row r="9" spans="1:42" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+    <row r="9" spans="1:42" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23" t="s">
+      <c r="B9" s="20"/>
+      <c r="C9" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23" t="s">
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23" t="s">
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="23"/>
-      <c r="R9" s="23"/>
-      <c r="S9" s="23"/>
-      <c r="T9" s="23"/>
-      <c r="U9" s="23" t="s">
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="20"/>
+      <c r="U9" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="V9" s="23"/>
-      <c r="W9" s="23"/>
-      <c r="X9" s="23"/>
-      <c r="Y9" s="23"/>
-      <c r="Z9" s="23"/>
-      <c r="AA9" s="23"/>
-      <c r="AB9" s="23"/>
-      <c r="AC9" s="23" t="s">
+      <c r="V9" s="20"/>
+      <c r="W9" s="20"/>
+      <c r="X9" s="20"/>
+      <c r="Y9" s="20"/>
+      <c r="Z9" s="20"/>
+      <c r="AA9" s="20"/>
+      <c r="AB9" s="20"/>
+      <c r="AC9" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="AD9" s="23"/>
-      <c r="AE9" s="23"/>
-      <c r="AF9" s="23"/>
-      <c r="AG9" s="23"/>
-      <c r="AH9" s="23"/>
-      <c r="AI9" s="23"/>
-      <c r="AJ9" s="23"/>
-      <c r="AK9" s="23" t="s">
+      <c r="AD9" s="20"/>
+      <c r="AE9" s="20"/>
+      <c r="AF9" s="20"/>
+      <c r="AG9" s="20"/>
+      <c r="AH9" s="20"/>
+      <c r="AI9" s="20"/>
+      <c r="AJ9" s="20"/>
+      <c r="AK9" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="AL9" s="23"/>
-      <c r="AM9" s="23"/>
-      <c r="AN9" s="23"/>
-      <c r="AO9" s="23"/>
-      <c r="AP9" s="23"/>
+      <c r="AL9" s="20"/>
+      <c r="AM9" s="20"/>
+      <c r="AN9" s="20"/>
+      <c r="AO9" s="20"/>
+      <c r="AP9" s="20"/>
     </row>
-    <row r="10" spans="1:42" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+    <row r="10" spans="1:42" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="27" t="s">
+      <c r="B10" s="20"/>
+      <c r="C10" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="27" t="s">
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="27" t="s">
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="23"/>
-      <c r="R10" s="23"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="23"/>
-      <c r="U10" s="28" t="s">
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="20"/>
+      <c r="U10" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="V10" s="23"/>
-      <c r="W10" s="23"/>
-      <c r="X10" s="23"/>
-      <c r="Y10" s="23"/>
-      <c r="Z10" s="23"/>
-      <c r="AA10" s="23"/>
-      <c r="AB10" s="23"/>
-      <c r="AC10" s="28" t="s">
+      <c r="V10" s="20"/>
+      <c r="W10" s="20"/>
+      <c r="X10" s="20"/>
+      <c r="Y10" s="20"/>
+      <c r="Z10" s="20"/>
+      <c r="AA10" s="20"/>
+      <c r="AB10" s="20"/>
+      <c r="AC10" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="AD10" s="23"/>
-      <c r="AE10" s="23"/>
-      <c r="AF10" s="23"/>
-      <c r="AG10" s="23"/>
-      <c r="AH10" s="23"/>
-      <c r="AI10" s="23"/>
-      <c r="AJ10" s="23"/>
-      <c r="AK10" s="28" t="s">
+      <c r="AD10" s="20"/>
+      <c r="AE10" s="20"/>
+      <c r="AF10" s="20"/>
+      <c r="AG10" s="20"/>
+      <c r="AH10" s="20"/>
+      <c r="AI10" s="20"/>
+      <c r="AJ10" s="20"/>
+      <c r="AK10" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="AL10" s="23"/>
-      <c r="AM10" s="23"/>
-      <c r="AN10" s="23"/>
-      <c r="AO10" s="23"/>
-      <c r="AP10" s="23"/>
+      <c r="AL10" s="20"/>
+      <c r="AM10" s="20"/>
+      <c r="AN10" s="20"/>
+      <c r="AO10" s="20"/>
+      <c r="AP10" s="20"/>
     </row>
-    <row r="11" spans="1:42" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
+    <row r="11" spans="1:42" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="29" t="s">
+      <c r="F11" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="N11" s="25" t="s">
+      <c r="N11" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="U11" s="25" t="s">
+      <c r="U11" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="AC11" s="25" t="s">
+      <c r="AC11" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="AK11" s="25" t="s">
+      <c r="AK11" s="22" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:42" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+    <row r="12" spans="1:42" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="24" t="s">
+      <c r="B12" s="20"/>
+      <c r="C12" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="24" t="s">
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="24" t="s">
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="23"/>
-      <c r="U12" s="24" t="s">
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="20"/>
+      <c r="T12" s="20"/>
+      <c r="U12" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="V12" s="23"/>
-      <c r="W12" s="23"/>
-      <c r="X12" s="23"/>
-      <c r="Y12" s="23"/>
-      <c r="Z12" s="23"/>
-      <c r="AA12" s="23"/>
-      <c r="AB12" s="23"/>
-      <c r="AC12" s="24" t="s">
+      <c r="V12" s="20"/>
+      <c r="W12" s="20"/>
+      <c r="X12" s="20"/>
+      <c r="Y12" s="20"/>
+      <c r="Z12" s="20"/>
+      <c r="AA12" s="20"/>
+      <c r="AB12" s="20"/>
+      <c r="AC12" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="AD12" s="23"/>
-      <c r="AE12" s="23"/>
-      <c r="AF12" s="23"/>
-      <c r="AG12" s="23"/>
-      <c r="AH12" s="23"/>
-      <c r="AI12" s="23"/>
-      <c r="AJ12" s="23"/>
-      <c r="AK12" s="23" t="b">
+      <c r="AD12" s="20"/>
+      <c r="AE12" s="20"/>
+      <c r="AF12" s="20"/>
+      <c r="AG12" s="20"/>
+      <c r="AH12" s="20"/>
+      <c r="AI12" s="20"/>
+      <c r="AJ12" s="20"/>
+      <c r="AK12" s="20" t="b">
         <v>1</v>
       </c>
-      <c r="AL12" s="23"/>
-      <c r="AM12" s="23"/>
-      <c r="AN12" s="23"/>
-      <c r="AO12" s="23"/>
-      <c r="AP12" s="23"/>
+      <c r="AL12" s="20"/>
+      <c r="AM12" s="20"/>
+      <c r="AN12" s="20"/>
+      <c r="AO12" s="20"/>
+      <c r="AP12" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2206,28 +2168,28 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9" t="s">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -2250,7 +2212,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -2273,7 +2235,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -2296,7 +2258,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -2319,13 +2281,13 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -2334,15 +2296,15 @@
       <c r="E8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -2365,36 +2327,36 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -2411,7 +2373,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -2434,70 +2396,66 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="12" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16" t="s">
+      <c r="A17" s="13"/>
+      <c r="C17" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="F17" t="s">
         <v>49</v>
       </c>
-      <c r="G17" s="17" t="s">
+      <c r="G17" s="14" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16" t="s">
+      <c r="A18" s="13"/>
+      <c r="D18" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16" t="s">
+      <c r="F18" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="17"/>
+      <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19" t="s">
+      <c r="A19" s="15"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="20"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>